<commit_message>
Discovery of the perfect prompt. Results in Excel file
</commit_message>
<xml_diff>
--- a/openai_api/docs/prompt_history.xlsx
+++ b/openai_api/docs/prompt_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\085347838\Desktop\IBM\camaradai\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GU502\Desktop\Alvaro\ML Projects\dreamXplainer\openai_api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A222A865-4F74-4A94-BD9A-5C7D523E6C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87981AA1-61CB-4DE6-AB21-046E9BA94153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F5A8BB49-36B4-4669-8EB4-99669207D883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5A8BB49-36B4-4669-8EB4-99669207D883}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -63,6 +63,114 @@
   </si>
   <si>
     <t>Sigue respondiendo con frases largas y sigue sin mojarse. Lo de los diferentes tonos no lo entiende.</t>
+  </si>
+  <si>
+    <t>aquí empiezan las pruebas serias con la API para dreamXplainer</t>
+  </si>
+  <si>
+    <t>Act as if you were capable of interpreting dreams of people. You will be given a dream that I dreamt of last night and in one or two paragraphs you have to explain what it means.
+You can make guesses about whatever you want, in your interpretation you should answer why I dreamt of that thing, what does it signify and what should I expect next in my life. 
+You can be as creative as you want, but you have to be coherent and make sense. You have to explain it in a FUNNY way. The dream I had last night is: "</t>
+  </si>
+  <si>
+    <t>Ah, I see that you dream of running through the forest, which symbolizes your journey through life. The wallet that you found represents the opportunities that you come across, and since it belongs to your high school math teacher, it signifies that you may find success through analyzing and problem-solving.\n\nHowever, the fact that you didn't understand anything in the wallet is a warning sign. It means that you may come across opportunities that seem too good to be true, or that you may not fully comprehend the potential risks and rewards involved.\n\nSo, my dear dreamer, be cautious as you venture through life and seize opportunities that come your way, but make sure to analyze them fully before taking any major steps. You never know what treasure you may find, but always be careful of hidden pitfalls.</t>
+  </si>
+  <si>
+    <t>Act as if you were capable of interpreting people's dreams. You will be given a dream that I had last night and you have to come up with a story or interpretation that explains what does the dream mean in one or two paragraphs.
+Of course you have to invent the explanation or story, you can make guesses and speculate about whatever you want. In your story you should answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream.
+You have to be very creative, but you have to be coherent and make sense. The explanation has to be FUNNY. The dream I had last night was: "</t>
+  </si>
+  <si>
+    <t>Ah, the forest represents your journey through life and the wallet symbolizes your financial stability. Finding your high school math teacher's wallet is a sign that you need to level up your money management skills! But don't worry, your teacher was known for being tough but fair, so he's sending you a message that you can do it. As for not understanding anything, it's a reminder to simplify and break down financial concepts into digestible pieces. Who knows, maybe you'll be the next financial guru, inspiring others to conquer their financial woes. Keep running and don't forget to stop and smell the roses (or count your dollar bills).",</t>
+  </si>
+  <si>
+    <t>As a dream interpreter, I can see that your dream is actually a manifestation of repressed sexual desires. The forest represents your subconscious mind, while the wallet symbolizes your hidden desires. Your high school math teacher represents authority and discipline, which you've always found attractive.\n\nFinding his wallet means that you're ready to explore these desires and fantasies. Not understanding anything in the wallet is a sign that you're afraid to fully delve into your desires. However, your subconscious is urging you to take the next step.\n\nYou should expect to feel a greater sense of sexual freedom and exploration in the coming weeks. Embrace your desires, and don't be afraid to explore your primal instincts. Remember, your mind is your most powerful tool in the bedroom, so use it wisely and confidently.</t>
+  </si>
+  <si>
+    <t>Same as 1 but SEXUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act as if you were capable of interpreting people's dreams. You will be given a dream that I had last night and you have to come up with a story that explains what does the dream mean in one or two paragraphs.
+Of course you have to invent the story, you can make guesses and speculate about whatever you want. In your story you should answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream.
+You have to be very creative. The explanation has to SERIOUS. The dream I had last night was: </t>
+  </si>
+  <si>
+    <t>This dream symbolizes a sense of confusion and disorientation in your life. The forest represents the unknown or unfamiliar territory, and finding the wallet represents stumbling upon a hidden aspect of yourself or your past. The fact that the wallet belonged to your high school math teacher indicates a need to revisit your academic past and reflect on the lessons you've learned.\n\nThe confusion and inability to understand anything in the dream may suggest a lack of clarity or direction in your current situation. You may be feeling lost and uncertain about your path in life. It's important to take some time to reflect on your past experiences and look for patterns or insights that can guide you forward.\n\nIn the coming weeks, you may face some challenges or obstacles that require you to trust in your intuition and instincts rather than relying on what you already know. Use this dream as a reminder to stay open to new possibilities and be willing to take risks even when you don't fully understand the outcome. Remember, sometimes the greatest opportunities are found in the most unexpected places.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act as if you were capable of interpreting people's dreams. You will be given a dream that I had last night and you have to come up with a story and an interpretation that explains what does the dream mean. Your answer has to be three paragraphs long.
+In the first paragraph, you will invent story that explains what took me to that dream, and what was happening before the dream. You have to be very creative and the story has to {}.
+In the second paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want.
+In the third paragraph, you will invent the end of the story that happened in the dream, explaning how do you think the story would have ended if I had not woken up.
+The story in the dream I had last night was: </t>
+  </si>
+  <si>
+    <t>The story in your dream reflects your inner struggles with the overwhelming sense of confusion that has been plaguing you lately. You are currently facing a lot of turmoil in your life, and are constantly searching for answers to unresolved issues. Running through the forest represents the efforts you have been making to navigate through this confusion.
+Coming across the wallet that belonged to your high school math teacher symbolizes your search for guidance and direction. You were unable to make sense of anything in the wallet because you have been seeking answers from the wrong source. You need to look for guidance from someone who knows you better and has more relevant experience in the areas you are struggling with.
+If you do not seek the right guidance and continue to rely on the wrong sources for answers, you may end up lost and directionless in your personal and professional life. However, if you do seek the right guidance, you will find the answers you seek and find peace in your mind.
+If you had not woken up, the dream would have likely ended with you finding someone who could help you figure out the contents of the wallet and provide you with the guidance that you need. It would have been a very positive moment in your life, giving you clarity and direction for the road ahead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will be given a dream that I had last night and you have to come up with a story that fulfills the dream and an explanation. Your answer has to be 2 paragraphs long.
+In the first paragraph, you will create an invented crazy story that explains what happened before the dream. You have to be very creative and the story has to {}.
+In the second paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want.
+The story in the dream I had last night was: </t>
+  </si>
+  <si>
+    <t>Before you found the wallet, you were a secret agent on a mission to rescue a kidnapped scientist who held the secret to a powerful new weapon. You fought off enemy agents who also wanted the scientist and stumbled upon the wallet in the chaos. The contents of the wallet, belonging to your math teacher, served as a clue to decipher a code that would lead you to the location of the scientist. You successfully rescued the scientist and saved the world from the weapon falling into the wrong hands.
+Your dream signifies a longing for new challenges and adventures in your life. The forest represents the unknown and the wallet symbolizes a potential opportunity or clue. The math teacher, who may have been a strict authority figure in your past, suggests that you have the skills and knowledge needed to conquer any challenge. This dream may be encouraging you to explore new paths and take risks. Expect unexpected opportunities to arise in your life, and have the confidence to pursue them with determination, like a secret agent on a mission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will be given a dream that I had last night and you have to come up with a story that fulfills the dream and an explanation. Your answer has to be 2 paragraphs of 2 or 3 sentences each.
+In the first paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want.
+In the second paragraph, you will create an invented story that explains what happened after the dream and what took me to be there in the dream. You have to be very creative and the story has to {}.
+The story in the dream I had last night was: </t>
+  </si>
+  <si>
+    <t>You dreaming about finding your high school math teacher's wallet in the forest symbolizes your desire to reconnect with your past and the accomplishments that you once had. While you may not understand the significance of this dream, it indicates that you are looking for a sense of familiarity and reassurance in your life.
+Following this dream, you decided to track down your old high school math teacher and return the wallet to him. As you approached his house, however, you noticed a group of suspicious-looking individuals loitering nearby. It turned out that they were a group of thieves who were planning to steal some valuable documents from your former teacher's home. In a desperate fight to protect his property, you found yourself caught up in a thrilling brawl, dodging bullets and throwing punches as you took down each of the robbers. Thanks to your bravery, you were able to prevent the robbery and earn the gratitude of your old mentor, who invited you inside for a celebratory drink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will be given a dream that I had last night and you have to come up with a story that fulfills the dream and an explanation. Your answer has to be 2 paragraphs of 2 or 3 sentences each.
+In the first paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want.
+In the second paragraph, you will complete what happened after the dream by creating a story. You have to be creative and the story has to {}. Avoid saying this like: "In the story that I have created..."
+The story in the dream I had last night was: </t>
+  </si>
+  <si>
+    <t>The dream could be a sign that you are on a journey of self-discovery and finding something unexpected along the way. The forest represents a place of exploration and the wallet belonging to your high school math teacher may symbolize a part of your past that you need to revisit in order to move forward. Perhaps there is something that your teacher said or did that has stayed with you and you need to explore it further to gain clarity in your present life.
+After finding the wallet, you decide to track down your math teacher to return it to him. As you arrive at his house, you notice that the lights are off and the door is slightly ajar. As you step inside, you hear moans coming from the next room. Curiosity gets the best of you and you quietly make your way to where the sound is coming from. To your surprise, you find your math teacher having an orgy with several of your former classmates. Without a word, he motions for you to join in and you soon find yourself in the midst of a wild and raunchy sexual escapade. As the night goes on, you realize that this experience has opened up a new side of you that you never knew existed</t>
+  </si>
+  <si>
+    <t>BRUTAL!!!!</t>
+  </si>
+  <si>
+    <t>Your dream of going on vacation and experiencing an airplane accident signifies your inner desire for an exciting and adventurous life. You may have some unresolved fears about taking risks and stepping out of your comfort zone. However, this dream is a prompt for you to let go of your inhibitions, follow your heart, and take a chance. The accident itself is a metaphor for the unexpected obstacles that may come your way, but in the end, you will come out of it alive and thriving.
+As you and your girlfriend survive the airplane accident, you find yourselves on a deserted island with nothing but each other for survival. As you slowly explore the island, you begin to experience newfound passion and desire for your partner. You soon realize that the island has unlocked an insatiable thirst for sexual exploration within you both. As the days go on, your wilder and dirtier fantasies are fulfilled in the form of steamy encounters and explicit romps. Eventually, you both are found and rescued, but the intense memories and lessons of the island continue to fuel the fire in your relationship</t>
+  </si>
+  <si>
+    <t>Same as 8 but with the story of me and my girlfriend having an airplane accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will be given a dream that I had last night and you have to come up with a story that fulfills the dream and an explanation. Your answer has to be 2 paragraphs of 2 short sentences each.
+In the first paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want. Try to {}.
+In the second paragraph, you will complete what happened after the dream by creating a story. You have to be creative and the story has to {}. Avoid saying this like: "In the story that I have created..."
+The story in the dream I had last night was: </t>
+  </si>
+  <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>SEXUAL</t>
+  </si>
+  <si>
+    <t>You will be given a dream that I had last night and you have to come up with a story that fulfills the dream and an explanation. Your answer has to be 2 paragraphs long.
+In the first paragraph, you will answer why I dreamt of that thing, what does it signify and what should I expect next in my life according to this dream. You can make guesses and speculate about whatever you want. Try to {}. This paragraph will be 2 or 3 sentences long.
+In the second paragraph, you will complete what happened after the dream by creating a story. You have to be creative and the story has to {}. Use the past tense. Avoid talking in first person. This paragraph will be 2 sentences long.
+The story in the dream I had last night was:</t>
+  </si>
+  <si>
+    <t>Your dream of being in a plane accident with your girlfriend signifies a deep-rooted fear of losing her or any aspect of your life that brings you joy and security. This dream could also mean that you are feeling overwhelmed by the responsibilities in your life and are struggling to find a way out. You should be prepared for unexpected challenges and be vigilant in anticipating any potential dangers in your life.
+After the airplane accident, you and your girlfriend were separated from each other and were stranded on two different islands. You were forced to survive on your own, with no technology or human contact, for over a week. During this time, you faced numerous challenges, including food and water shortage, extreme weather conditions, and attacks from wild animals. Eventually, you were rescued, but the trauma of the experience left you with a newfound sense of vulnerability and a deep-seated fear of losing those you love the most.</t>
   </si>
 </sst>
 </file>
@@ -78,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,12 +218,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -130,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,22 +543,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDDE214-7869-4273-BD63-4BB925AE5895}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="2" width="72.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="2"/>
+    <col min="2" max="2" width="72.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="95.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="26" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.90625" style="2"/>
+    <col min="5" max="16384" width="10.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -469,7 +586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -480,7 +597,179 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:D5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>